<commit_message>
more fucking cleaning in Henriette shit
</commit_message>
<xml_diff>
--- a/data/extractions/250527 Fiche d'extraction d'échantillons.xlsx
+++ b/data/extractions/250527 Fiche d'extraction d'échantillons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itgitm-my.sharepoint.com/personal/nvanreet_itg_be/Documents/Documenten/GitHub/biobank-dashboard/data/extractions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1EE8AD49-17A5-4AFC-8EF2-5DD0EBF7F026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57A9069F-36DF-4396-B9B7-E8AC869AB3E9}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1EE8AD49-17A5-4AFC-8EF2-5DD0EBF7F026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DC5CE68-98FC-4411-BA46-948EB7ACF335}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1CE68EB6-DB45-45E9-95B2-F2EDACD56A3B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>Numéro</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>DIEUD0</t>
   </si>
   <si>
     <t>C</t>
@@ -649,7 +646,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,16 +726,16 @@
         <v>45804</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="L2" s="2">
         <v>5</v>
@@ -767,16 +764,16 @@
         <v>45804</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="L3" s="2">
         <v>6</v>
@@ -805,16 +802,16 @@
         <v>45804</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="L4" s="2">
         <v>7</v>
@@ -843,16 +840,16 @@
         <v>45804</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="L5" s="2">
         <v>8</v>
@@ -881,16 +878,16 @@
         <v>45804</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="L6" s="2">
         <v>9</v>
@@ -919,16 +916,16 @@
         <v>45804</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="L7" s="2">
         <v>10</v>
@@ -957,16 +954,16 @@
         <v>45804</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="L8" s="2">
         <v>11</v>
@@ -995,16 +992,16 @@
         <v>45804</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="L9" s="2">
         <v>12</v>
@@ -1033,16 +1030,16 @@
         <v>45804</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="L10" s="2">
         <v>1</v>
@@ -1071,16 +1068,16 @@
         <v>45804</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="L11" s="2">
         <v>2</v>
@@ -1094,6 +1091,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Uploaded xmlns="974e1998-2087-4290-81d3-cf83f1cc5cbf">2025-05-30T10:47:20+00:00</Uploaded>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005F56A3FBA1F9FF429D4C886089ACEF10" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="9259fe1b952dc853dcaf14f7078ccc22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="974e1998-2087-4290-81d3-cf83f1cc5cbf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11627f76d2a82a971f29bd5674bd7693" ns2:_="">
     <xsd:import namespace="974e1998-2087-4290-81d3-cf83f1cc5cbf"/>
@@ -1237,24 +1251,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C8D065-0006-41F8-8E7D-21E3F4FEEF2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="974e1998-2087-4290-81d3-cf83f1cc5cbf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Uploaded xmlns="974e1998-2087-4290-81d3-cf83f1cc5cbf">2025-05-30T10:47:20+00:00</Uploaded>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BD5A77D-2C96-4809-A195-F2AA12C1040C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA6493F8-46F4-4D28-8210-16CCA6DE286E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1270,22 +1285,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BD5A77D-2C96-4809-A195-F2AA12C1040C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C8D065-0006-41F8-8E7D-21E3F4FEEF2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="974e1998-2087-4290-81d3-cf83f1cc5cbf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>